<commit_message>
adding a settings icon
</commit_message>
<xml_diff>
--- a/component library/icons/webfont/icon font list.xlsx
+++ b/component library/icons/webfont/icon font list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14740" windowHeight="16060" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>less</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>circleCheck</t>
+  </si>
+  <si>
+    <t>settings</t>
   </si>
 </sst>
 </file>
@@ -538,7 +541,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -847,6 +850,9 @@
       <c r="A28">
         <v>61453</v>
       </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
       <c r="C28" t="str">
         <f t="shared" si="3"/>
         <v>F00D</v>

</xml_diff>

<commit_message>
new icons for download and share
</commit_message>
<xml_diff>
--- a/component library/icons/webfont/icon font list.xlsx
+++ b/component library/icons/webfont/icon font list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14740" windowHeight="16060" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>less</t>
   </si>
@@ -112,6 +112,18 @@
   </si>
   <si>
     <t>settings</t>
+  </si>
+  <si>
+    <t>download</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>details</t>
+  </si>
+  <si>
+    <t>item-settings</t>
   </si>
 </sst>
 </file>
@@ -541,7 +553,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -889,6 +901,9 @@
       <c r="A32">
         <v>61457</v>
       </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
       <c r="C32" t="str">
         <f t="shared" si="4"/>
         <v>F011</v>
@@ -898,6 +913,9 @@
       <c r="A33">
         <v>61458</v>
       </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
       <c r="C33" t="str">
         <f t="shared" si="4"/>
         <v>F012</v>
@@ -907,6 +925,9 @@
       <c r="A34">
         <v>61459</v>
       </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
       <c r="C34" t="str">
         <f t="shared" si="4"/>
         <v>F013</v>
@@ -915,6 +936,9 @@
     <row r="35" spans="1:3">
       <c r="A35">
         <v>61460</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" ref="C35:C44" si="5">DEC2HEX(A35, 4)</f>

</xml_diff>